<commit_message>
updated elec files to adjust for CHP
</commit_message>
<xml_diff>
--- a/InputData/elec/GDPbES/Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/GDPbES/Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/elec/gdpbes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\GDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1D2D8E-8901-B44D-9456-EC10F70F5549}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED7F9D8-C7F8-46DF-AC31-EDD8F4A510C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="23000" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8220" yWindow="1140" windowWidth="16275" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -524,11 +524,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -536,77 +536,77 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -624,15 +624,17 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -745,7 +747,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -893,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1041,7 +1043,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1189,7 +1191,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1337,7 +1339,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1485,7 +1487,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1633,7 +1635,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1929,7 +1931,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2077,7 +2079,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2225,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2521,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2669,156 +2671,120 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
       <c r="B15">
-        <f>B11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:AK15" si="3">C11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ15">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2827,147 +2793,147 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" ref="C16:AK16" si="4">C11</f>
+        <f t="shared" ref="C16:AK16" si="3">C11</f>
         <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK16">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2976,143 +2942,143 @@
         <v>0.5</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:AK17" si="5">C9</f>
+        <f t="shared" ref="C17:AK17" si="4">C9</f>
         <v>0.5</v>
       </c>
       <c r="D17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="E17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="F17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="G17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="H17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="I17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="J17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="K17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="L17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="M17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="N17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="P17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="R17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="S17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="T17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="U17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="V17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="W17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="X17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AF17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AH17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AI17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AJ17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AK17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
     </row>

</xml_diff>